<commit_message>
Added google sheets support
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -76,10 +76,10 @@
     <t xml:space="preserve">Рамен на насыщенном сырном бульоне на основе кокосового молока, с добавлением куриной грудинки, яично - пшеничной лапши, мисо-матадоре, ростков зелени, листьев вакамэ</t>
   </si>
   <si>
-    <t xml:space="preserve">Тестовый Рамен</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рамен, который потестирован и что-то работает</t>
+    <t xml:space="preserve">Тестовый Рамен 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рамен, который потестирован и что-то работает, незаметно подменил</t>
   </si>
   <si>
     <t xml:space="preserve">Алкогольное меню</t>
@@ -280,7 +280,7 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -288,7 +288,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="54.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="47.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11"/>
   </cols>

</xml_diff>